<commit_message>
prediction(): predict animacy of words with particular attribute.
</commit_message>
<xml_diff>
--- a/extracted_nouns/BNC/nouns_bnc+lbl+key+ani_mid.xlsx
+++ b/extracted_nouns/BNC/nouns_bnc+lbl+key+ani_mid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iojdw\Research\extracted_nouns\BNC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB37241B-3DCF-400E-90CA-A4C318AD03A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5564E2-FEAF-47C9-9C78-36187E055D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21525" yWindow="2775" windowWidth="14400" windowHeight="7275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="649">
   <si>
     <t>people</t>
   </si>
@@ -1984,19 +1984,6 @@
     </rPh>
     <rPh sb="4" eb="7">
       <t>ユウセイブツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>神・精霊・霊魂</t>
-    <rPh sb="0" eb="1">
-      <t>カミ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>セイレイ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>レイコン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2039,6 +2026,36 @@
     <rPh sb="3" eb="6">
       <t>ビセイブツ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>←ここからplant/collective/spirit/brainのみラベル付け</t>
+    <rPh sb="39" eb="40">
+      <t>ヅ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>神・精霊・霊魂・天使・空想のもの</t>
+    <rPh sb="0" eb="1">
+      <t>カミ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>セイレイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>レイコン</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>テンシ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>クウソウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>special</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5369,11 +5386,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I263"/>
+  <dimension ref="A1:J263"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G264" sqref="G264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -5389,7 +5406,7 @@
     <col min="9" max="9" width="5.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>631</v>
       </c>
@@ -5400,7 +5417,7 @@
         <v>633</v>
       </c>
       <c r="D1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E1" t="s">
         <v>636</v>
@@ -5415,10 +5432,13 @@
         <v>639</v>
       </c>
       <c r="I1" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>644</v>
+      </c>
+      <c r="J1" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>369</v>
       </c>
@@ -5432,7 +5452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>370</v>
       </c>
@@ -5446,7 +5466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>371</v>
       </c>
@@ -5460,7 +5480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>372</v>
       </c>
@@ -5477,7 +5497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>373</v>
       </c>
@@ -5488,7 +5508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>374</v>
       </c>
@@ -5505,7 +5525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>375</v>
       </c>
@@ -5516,7 +5536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>376</v>
       </c>
@@ -5527,7 +5547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>377</v>
       </c>
@@ -5538,7 +5558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>378</v>
       </c>
@@ -5549,7 +5569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>379</v>
       </c>
@@ -5560,7 +5580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>380</v>
       </c>
@@ -5574,7 +5594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>381</v>
       </c>
@@ -5591,7 +5611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>382</v>
       </c>
@@ -5602,7 +5622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>383</v>
       </c>
@@ -5619,7 +5639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>384</v>
       </c>
@@ -5633,7 +5653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>385</v>
       </c>
@@ -5647,7 +5667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>386</v>
       </c>
@@ -5658,7 +5678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>387</v>
       </c>
@@ -5669,7 +5689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>388</v>
       </c>
@@ -5683,7 +5703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>389</v>
       </c>
@@ -5697,7 +5717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>390</v>
       </c>
@@ -5711,7 +5731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>391</v>
       </c>
@@ -5725,7 +5745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>392</v>
       </c>
@@ -5742,7 +5762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>393</v>
       </c>
@@ -5756,7 +5776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>394</v>
       </c>
@@ -5764,7 +5784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>395</v>
       </c>
@@ -5775,7 +5795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>396</v>
       </c>
@@ -5789,7 +5809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>397</v>
       </c>
@@ -5803,7 +5823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>398</v>
       </c>
@@ -5817,15 +5837,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>399</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J32" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>400</v>
       </c>
@@ -5833,7 +5856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>401</v>
       </c>
@@ -5841,7 +5864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>402</v>
       </c>
@@ -5849,55 +5872,79 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>403</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>404</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>405</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>406</v>
       </c>
       <c r="B39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>407</v>
       </c>
       <c r="B40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>408</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>409</v>
       </c>
@@ -5905,47 +5952,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>410</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>411</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>412</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>413</v>
       </c>
       <c r="B46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>414</v>
       </c>
       <c r="B47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>415</v>
       </c>
@@ -5953,31 +6015,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>416</v>
       </c>
       <c r="B49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>417</v>
       </c>
       <c r="B50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>418</v>
       </c>
       <c r="B51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>419</v>
       </c>
@@ -5985,47 +6056,65 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>420</v>
       </c>
       <c r="B53">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>421</v>
       </c>
       <c r="B54">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>422</v>
       </c>
       <c r="B55">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>423</v>
       </c>
       <c r="B56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>424</v>
       </c>
       <c r="B57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>425</v>
       </c>
@@ -6033,15 +6122,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>426</v>
       </c>
       <c r="B59">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>427</v>
       </c>
@@ -6049,7 +6141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>428</v>
       </c>
@@ -6057,7 +6149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>429</v>
       </c>
@@ -6065,15 +6157,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>430</v>
       </c>
       <c r="B63">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>431</v>
       </c>
@@ -6081,15 +6176,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>432</v>
       </c>
       <c r="B65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>433</v>
       </c>
@@ -6097,7 +6195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>434</v>
       </c>
@@ -6105,7 +6203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>435</v>
       </c>
@@ -6113,7 +6211,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>436</v>
       </c>
@@ -6121,15 +6219,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>437</v>
       </c>
       <c r="B70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>438</v>
       </c>
@@ -6137,7 +6238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>439</v>
       </c>
@@ -6145,31 +6246,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>440</v>
       </c>
       <c r="B73">
         <v>2</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>441</v>
       </c>
       <c r="B74">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>442</v>
       </c>
       <c r="B75">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>443</v>
       </c>
@@ -6177,15 +6287,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>444</v>
       </c>
       <c r="B77">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>445</v>
       </c>
@@ -6193,7 +6306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>446</v>
       </c>
@@ -6201,15 +6314,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>447</v>
       </c>
       <c r="B80">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>448</v>
       </c>
@@ -6217,7 +6333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>449</v>
       </c>
@@ -6225,7 +6341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>450</v>
       </c>
@@ -6233,15 +6349,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>451</v>
       </c>
       <c r="B84">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>452</v>
       </c>
@@ -6249,7 +6368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>453</v>
       </c>
@@ -6257,15 +6376,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>454</v>
       </c>
       <c r="B87">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>455</v>
       </c>
@@ -6273,7 +6395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>456</v>
       </c>
@@ -6281,7 +6403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>457</v>
       </c>
@@ -6289,15 +6411,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+    <row r="91" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="B91">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B91" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>459</v>
       </c>
@@ -6305,7 +6427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>460</v>
       </c>
@@ -6313,7 +6435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>461</v>
       </c>
@@ -6321,7 +6443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>462</v>
       </c>
@@ -6329,23 +6451,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>463</v>
       </c>
       <c r="B96">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>464</v>
       </c>
       <c r="B97">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>465</v>
       </c>
@@ -6353,7 +6481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>466</v>
       </c>
@@ -6361,15 +6489,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>467</v>
       </c>
       <c r="B100">
         <v>2</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>468</v>
       </c>
@@ -6377,7 +6508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>469</v>
       </c>
@@ -6385,15 +6516,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>470</v>
       </c>
       <c r="B103">
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>471</v>
       </c>
@@ -6401,23 +6535,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>472</v>
       </c>
       <c r="B105">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>473</v>
       </c>
       <c r="B106">
         <v>2</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>474</v>
       </c>
@@ -6425,7 +6565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>475</v>
       </c>
@@ -6433,15 +6573,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>476</v>
       </c>
       <c r="B109">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>477</v>
       </c>
@@ -6449,7 +6592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>478</v>
       </c>
@@ -6457,7 +6600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>479</v>
       </c>
@@ -6465,7 +6608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>480</v>
       </c>
@@ -6473,15 +6616,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>481</v>
       </c>
       <c r="B114">
         <v>2</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>482</v>
       </c>
@@ -6489,15 +6635,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>483</v>
       </c>
       <c r="B116">
         <v>2</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>484</v>
       </c>
@@ -6505,7 +6654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>485</v>
       </c>
@@ -6513,23 +6662,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>486</v>
       </c>
       <c r="B119">
         <v>2</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>487</v>
       </c>
       <c r="B120">
         <v>2</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>488</v>
       </c>
@@ -6537,7 +6692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>489</v>
       </c>
@@ -6545,15 +6700,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>490</v>
       </c>
       <c r="B123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>491</v>
       </c>
@@ -6561,7 +6719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>492</v>
       </c>
@@ -6569,7 +6727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>493</v>
       </c>
@@ -6577,7 +6735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>494</v>
       </c>
@@ -6585,7 +6743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>495</v>
       </c>
@@ -6593,7 +6751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>496</v>
       </c>
@@ -6601,7 +6759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>497</v>
       </c>
@@ -6609,15 +6767,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>498</v>
       </c>
       <c r="B131">
         <v>2</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>499</v>
       </c>
@@ -6625,7 +6786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>500</v>
       </c>
@@ -6633,23 +6794,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>501</v>
       </c>
       <c r="B134">
         <v>2</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>502</v>
       </c>
       <c r="B135">
         <v>2</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>503</v>
       </c>
@@ -6657,7 +6824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>504</v>
       </c>
@@ -6665,7 +6832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>505</v>
       </c>
@@ -6673,7 +6840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>506</v>
       </c>
@@ -6681,15 +6848,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>507</v>
       </c>
       <c r="B140">
         <v>2</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>508</v>
       </c>
@@ -6697,7 +6867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>509</v>
       </c>
@@ -6705,15 +6875,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>510</v>
       </c>
       <c r="B143">
         <v>2</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>511</v>
       </c>
@@ -6721,7 +6894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>512</v>
       </c>
@@ -6729,31 +6902,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>513</v>
       </c>
       <c r="B146">
         <v>2</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>514</v>
       </c>
       <c r="B147">
         <v>2</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>515</v>
       </c>
       <c r="B148">
         <v>2</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>516</v>
       </c>
@@ -6761,7 +6943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>517</v>
       </c>
@@ -6769,15 +6951,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>518</v>
       </c>
       <c r="B151">
         <v>2</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>519</v>
       </c>
@@ -6785,23 +6970,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>520</v>
       </c>
       <c r="B153">
         <v>2</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>521</v>
       </c>
       <c r="B154">
         <v>2</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>522</v>
       </c>
@@ -6809,55 +7000,73 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>523</v>
       </c>
       <c r="B156">
         <v>2</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>524</v>
       </c>
       <c r="B157">
         <v>2</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>525</v>
       </c>
       <c r="B158">
         <v>2</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>526</v>
       </c>
       <c r="B159">
         <v>2</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>527</v>
       </c>
       <c r="B160">
         <v>2</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>528</v>
       </c>
       <c r="B161">
         <v>2</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>529</v>
       </c>
@@ -6865,7 +7074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>530</v>
       </c>
@@ -6873,7 +7082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>531</v>
       </c>
@@ -6881,15 +7090,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>532</v>
       </c>
       <c r="B165">
         <v>2</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>533</v>
       </c>
@@ -6897,7 +7109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>534</v>
       </c>
@@ -6905,7 +7117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>535</v>
       </c>
@@ -6913,7 +7125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>536</v>
       </c>
@@ -6921,15 +7133,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>537</v>
       </c>
       <c r="B170">
         <v>2</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>538</v>
       </c>
@@ -6937,7 +7152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>539</v>
       </c>
@@ -6945,15 +7160,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>540</v>
       </c>
       <c r="B173">
         <v>2</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>541</v>
       </c>
@@ -6961,7 +7179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>542</v>
       </c>
@@ -6969,15 +7187,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>543</v>
       </c>
       <c r="B176">
         <v>2</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>544</v>
       </c>
@@ -6985,7 +7206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>545</v>
       </c>
@@ -6993,23 +7214,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>546</v>
       </c>
       <c r="B179">
         <v>2</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>547</v>
       </c>
       <c r="B180">
         <v>2</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>548</v>
       </c>
@@ -7017,7 +7244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>549</v>
       </c>
@@ -7025,15 +7252,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>550</v>
       </c>
       <c r="B183">
         <v>2</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>551</v>
       </c>
@@ -7041,7 +7271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>552</v>
       </c>
@@ -7049,7 +7279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>553</v>
       </c>
@@ -7057,15 +7287,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>554</v>
       </c>
       <c r="B187">
         <v>2</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>555</v>
       </c>
@@ -7073,7 +7306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>556</v>
       </c>
@@ -7081,7 +7314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>557</v>
       </c>
@@ -7089,7 +7322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>558</v>
       </c>
@@ -7097,7 +7330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>559</v>
       </c>
@@ -7105,47 +7338,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>560</v>
       </c>
       <c r="B193">
         <v>2</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>561</v>
       </c>
       <c r="B194">
         <v>2</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>562</v>
       </c>
       <c r="B195">
         <v>2</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>563</v>
       </c>
       <c r="B196">
         <v>2</v>
       </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>564</v>
       </c>
       <c r="B197">
         <v>2</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>565</v>
       </c>
@@ -7153,15 +7401,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>566</v>
       </c>
       <c r="B199">
         <v>2</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>567</v>
       </c>
@@ -7169,7 +7420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>568</v>
       </c>
@@ -7177,31 +7428,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>569</v>
       </c>
       <c r="B202">
         <v>2</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>570</v>
       </c>
       <c r="B203">
         <v>2</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>571</v>
       </c>
       <c r="B204">
         <v>2</v>
       </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>572</v>
       </c>
@@ -7209,23 +7469,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>573</v>
       </c>
       <c r="B206">
         <v>2</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F206">
+        <v>1</v>
+      </c>
+      <c r="G206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>574</v>
       </c>
       <c r="B207">
         <v>2</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>575</v>
       </c>
@@ -7233,31 +7502,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>576</v>
       </c>
       <c r="B209">
         <v>2</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>577</v>
       </c>
       <c r="B210">
         <v>2</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>578</v>
       </c>
       <c r="B211">
         <v>2</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>579</v>
       </c>
@@ -7265,7 +7543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>580</v>
       </c>
@@ -7273,7 +7551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>581</v>
       </c>
@@ -7281,7 +7559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>582</v>
       </c>
@@ -7289,23 +7567,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>583</v>
       </c>
       <c r="B216">
         <v>2</v>
       </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>584</v>
       </c>
       <c r="B217">
         <v>2</v>
       </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>585</v>
       </c>
@@ -7313,15 +7597,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>586</v>
       </c>
       <c r="B219">
         <v>2</v>
       </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>587</v>
       </c>
@@ -7329,15 +7616,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>588</v>
       </c>
       <c r="B221">
         <v>2</v>
       </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>589</v>
       </c>
@@ -7345,7 +7635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>590</v>
       </c>
@@ -7353,7 +7643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>591</v>
       </c>
@@ -7361,15 +7651,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>592</v>
       </c>
       <c r="B225">
         <v>2</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>593</v>
       </c>
@@ -7377,15 +7670,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>594</v>
       </c>
       <c r="B227">
         <v>2</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>595</v>
       </c>
@@ -7393,7 +7689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>596</v>
       </c>
@@ -7401,7 +7697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>597</v>
       </c>
@@ -7409,7 +7705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>598</v>
       </c>
@@ -7417,39 +7713,51 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>599</v>
       </c>
       <c r="B232">
         <v>2</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>600</v>
       </c>
       <c r="B233">
         <v>2</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>601</v>
       </c>
       <c r="B234">
         <v>2</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>602</v>
       </c>
       <c r="B235">
         <v>2</v>
       </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>603</v>
       </c>
@@ -7457,7 +7765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>604</v>
       </c>
@@ -7465,7 +7773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>605</v>
       </c>
@@ -7473,7 +7781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>606</v>
       </c>
@@ -7481,7 +7789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>607</v>
       </c>
@@ -7489,7 +7797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>608</v>
       </c>
@@ -7497,7 +7805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>609</v>
       </c>
@@ -7505,7 +7813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>610</v>
       </c>
@@ -7513,7 +7821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>611</v>
       </c>
@@ -7521,7 +7829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>612</v>
       </c>
@@ -7529,23 +7837,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>613</v>
       </c>
       <c r="B246">
         <v>2</v>
       </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>614</v>
       </c>
       <c r="B247">
         <v>2</v>
       </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>615</v>
       </c>
@@ -7553,15 +7867,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>616</v>
       </c>
       <c r="B249">
         <v>2</v>
       </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>617</v>
       </c>
@@ -7569,7 +7886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>618</v>
       </c>
@@ -7577,15 +7894,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>619</v>
       </c>
       <c r="B252">
         <v>2</v>
       </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>620</v>
       </c>
@@ -7593,7 +7913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>621</v>
       </c>
@@ -7601,15 +7921,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>622</v>
       </c>
       <c r="B255">
         <v>2</v>
       </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>623</v>
       </c>
@@ -7617,7 +7940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>624</v>
       </c>
@@ -7625,7 +7948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>625</v>
       </c>
@@ -7633,15 +7956,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>626</v>
       </c>
       <c r="B259">
         <v>2</v>
       </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>627</v>
       </c>
@@ -7649,7 +7975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>628</v>
       </c>
@@ -7657,7 +7983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>629</v>
       </c>
@@ -7665,12 +7991,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>630</v>
       </c>
       <c r="B263">
         <v>2</v>
+      </c>
+      <c r="G263">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7683,7 +8012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C54B64A-C8FF-4821-8FEC-61BDD7D43A87}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -7697,10 +8028,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>642</v>
+      </c>
+      <c r="B2" t="s">
         <v>643</v>
-      </c>
-      <c r="B2" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -7724,7 +8055,7 @@
         <v>638</v>
       </c>
       <c r="B5" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -7732,15 +8063,15 @@
         <v>639</v>
       </c>
       <c r="B6" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>644</v>
+      </c>
+      <c r="B7" t="s">
         <v>645</v>
-      </c>
-      <c r="B7" t="s">
-        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>